<commit_message>
Wrangled CLR, fixed date and subject values
</commit_message>
<xml_diff>
--- a/mss0048/CLR/CLR_small_manu_mss0048.xlsx
+++ b/mss0048/CLR/CLR_small_manu_mss0048.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\small_manuscript_collections\mss0048\CLR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\domm-metadata\mss0048\CLR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="648">
   <si>
     <t>text</t>
   </si>
@@ -2059,13 +2059,7 @@
     <t>001</t>
   </si>
   <si>
-    <t>mss0048CLR.tiff</t>
-  </si>
-  <si>
     <t>Chapman Family Correspondence and Other Documents</t>
-  </si>
-  <si>
-    <t>Chapman family|Chapman, J. G. (John Gadsby), 1808-1889|Chapman, Conrad Wise, 1842-1910</t>
   </si>
   <si>
     <t>1791-1898, bulk 1861-1865</t>
@@ -2081,16 +2075,37 @@
     <t>From the &lt;a href="http://libraries.ucsd.edu/speccoll/findingaids/mss0048.html"&gt;Chapman Family Correspondence and Other Documents&lt;/a&gt;. MSS 48. Special Collections &amp; Archives, UC San Diego.</t>
   </si>
   <si>
-    <t>Chapman, J. G. (John Gadsby), 1808-1889 -- Correspondence|Chapman, Conrad Wise, 1842-1910 -- Correspondence</t>
-  </si>
-  <si>
-    <t>United States -- History -- Civil War, 1861-1865 -- Personal narratives, Confederate</t>
-  </si>
-  <si>
-    <t>Confederate States of America. Army|Painters -- America -- Manuscripts|American Civil War (1861-1865)|History -- Sources</t>
-  </si>
-  <si>
     <t>Chapman Family Correspondence and Other Documents @ http://libraries.ucsd.edu/speccoll/findingaids/mss0048.html</t>
+  </si>
+  <si>
+    <t>mss0048CLR.tif</t>
+  </si>
+  <si>
+    <t>Chapman family | Chapman, J. G. (John Gadsby), 1808-1889 | Chapman, Conrad Wise, 1842-1910</t>
+  </si>
+  <si>
+    <t>1791-01-01</t>
+  </si>
+  <si>
+    <t>1898-12-31</t>
+  </si>
+  <si>
+    <t>Confederate States of America. Army</t>
+  </si>
+  <si>
+    <t>Chapman, J. G. (John Gadsby), 1808-1889 | Chapman, Conrad Wise, 1842-1910</t>
+  </si>
+  <si>
+    <t>Personal narratives--Confederate</t>
+  </si>
+  <si>
+    <t>Manuscripts</t>
+  </si>
+  <si>
+    <t>Painters | Painters--Correspondence | American Civil War (1861-1865) | History--Sources</t>
+  </si>
+  <si>
+    <t>Chapman family</t>
   </si>
 </sst>
 </file>
@@ -3136,9 +3151,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -3155,11 +3170,11 @@
     <col min="9" max="9" width="15.140625" style="3" customWidth="1"/>
     <col min="10" max="10" width="19.85546875" style="3" customWidth="1"/>
     <col min="11" max="12" width="39.140625" style="3" customWidth="1"/>
-    <col min="13" max="15" width="42.85546875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="84.28515625" style="3" customWidth="1"/>
+    <col min="13" max="18" width="42.85546875" style="3" customWidth="1"/>
+    <col min="19" max="19" width="84.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>337</v>
       </c>
@@ -3200,21 +3215,30 @@
         <v>458</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>454</v>
+        <v>336</v>
       </c>
       <c r="O1" s="16" t="s">
         <v>459</v>
       </c>
       <c r="P1" s="16" t="s">
+        <v>459</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>450</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="S1" s="16" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>631</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>632</v>
+        <v>638</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -3223,40 +3247,49 @@
         <v>357</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="G2" s="23" t="s">
         <v>633</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="23" t="s">
+        <v>640</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>641</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="K2" s="3" t="s">
         <v>635</v>
       </c>
-      <c r="H2" s="23">
-        <v>1791</v>
-      </c>
-      <c r="I2" s="23">
-        <v>1898</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>636</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>637</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>638</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>639</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>640</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -3297,7 +3330,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>P1</xm:sqref>
+          <xm:sqref>S1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
@@ -3315,7 +3348,7 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>M1:O1</xm:sqref>
+          <xm:sqref>M1:N1 O1:R1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>